<commit_message>
dodanie przypadków dot. zmiany hasła
</commit_message>
<xml_diff>
--- a/PrzypadkiUżycia.xlsx
+++ b/PrzypadkiUżycia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="101">
   <si>
     <t>numer ID</t>
   </si>
@@ -361,7 +361,67 @@
 2. Kliknij przycisk "Dodaj do koszyka".</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>ID 0017</t>
+  </si>
+  <si>
+    <t>ID 0018</t>
+  </si>
+  <si>
+    <t>ID 0019</t>
+  </si>
+  <si>
+    <t>ID 0020</t>
+  </si>
+  <si>
+    <t>Komunikat o niepoprawnym wypełnieniu pola "Użytkownik lub e-mail".</t>
+  </si>
+  <si>
+    <t>Przekierowanie na stronę profilu użytkownika. Otrzymanie maila z wygenerowanym hasłem.</t>
+  </si>
+  <si>
+    <t>Użytkownik musi być zalogowany.
+ Użytkownik znajduje się na stronie głównej sklepu www.pocztaksiazkowa.pl</t>
+  </si>
+  <si>
+    <t>Hasło zostało zmienione.</t>
+  </si>
+  <si>
+    <t>Komunikat o pozytywnej zmianie szczegółów konta.</t>
+  </si>
+  <si>
+    <t>Poprawna zmiana hasła użytkownika.</t>
+  </si>
+  <si>
+    <t>Celem testu jest sprawdzenie zachowania się systemu przy próbie zmiany hasła na zbyt krótkie.</t>
+  </si>
+  <si>
+    <t>Hasło nie zostało zmienione.</t>
+  </si>
+  <si>
+    <t>System nie podejmuje akcji zmiany ustawień konta. Pod polem "Nowe hasło" pojawia się komunikat z informacją, jak powinno wygladać poprawne hasło.</t>
+  </si>
+  <si>
+    <t>Próba zmiany hasła na nieprawidłowe.</t>
+  </si>
+  <si>
+    <t>Celem testu jest zmiana hasła przy zachowaniu prawidłowej jego długości.</t>
+  </si>
+  <si>
+    <t>1. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Szczegóły konta".
+3. W polu "Aktualne hasło" wpisz hasło otrzymane na maila wraz z mailem potwierdzającym rejestrację lub swoje zmienione hasło.
+4. W polu "Nowe hasło" wpisz hasło składające się z conajmniej 12 znaków.
+5. Powtórz hasło w polu "Potwierdź nowe hasło".
+6. Jeśli jest to pierwsza zmiana hasła po zarejestrowaniu użytkownika to należy także wypełnić puste pola "Imię" oraz "Nazwisko".
+7. Kliknij przycisk "zapisz zmiany".</t>
+  </si>
+  <si>
+    <t>2. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Szczegóły konta".
+3. W polu "Aktualne hasło" wpisz hasło otrzymane na maila wraz z mailem potwierdzającym rejestrację lub swoje zmienione hasło.
+4. W polu "Nowe hasło" wpisz hasło zawierające mniej niż 12 znaków.
+5. Powtórz hasło w polu "Potwierdź nowe hasło".
+6. Kliknij przycisk "Zapisz zmiany".</t>
   </si>
 </sst>
 </file>
@@ -428,7 +488,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -452,6 +512,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -461,7 +536,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -470,13 +545,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -488,10 +578,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -503,10 +591,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -518,10 +604,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -533,8 +617,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -546,8 +632,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -559,8 +647,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -572,12 +662,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -587,91 +675,110 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,582 +1074,642 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13:J14"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="7.25" customWidth="1"/>
     <col min="2" max="2" width="10.875" customWidth="1"/>
-    <col min="3" max="3" width="18.25" customWidth="1"/>
-    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="21.125" customWidth="1"/>
-    <col min="7" max="7" width="22.25" customWidth="1"/>
-    <col min="8" max="8" width="34.375" customWidth="1"/>
-    <col min="9" max="9" width="19.875" customWidth="1"/>
+    <col min="6" max="6" width="26.75" customWidth="1"/>
+    <col min="7" max="7" width="27.625" customWidth="1"/>
+    <col min="8" max="8" width="58.125" customWidth="1"/>
+    <col min="9" max="9" width="23.625" customWidth="1"/>
     <col min="10" max="10" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="98.25" customHeight="1">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:10" ht="63" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="77.25" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="78.75" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="81.75" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="79.5" customHeight="1">
+      <c r="A6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="96" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="107.25" customHeight="1">
-      <c r="A3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="J7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="95.25" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="13" t="s">
+      <c r="F8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="140.25" customHeight="1">
-      <c r="A4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="H8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="95.25" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="13" t="s">
+      <c r="F9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="108.75" customHeight="1">
-      <c r="A5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="H9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="95.25" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="F10" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="119.25" customHeight="1">
-      <c r="A6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="H10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="155.25" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="108.75" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="13" t="s">
+      <c r="F12" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="123.75" customHeight="1">
-      <c r="A7" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="H12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30">
+      <c r="A13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" ht="30">
+      <c r="A14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="30">
+      <c r="A15" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="30">
+      <c r="A16" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" ht="30">
+      <c r="A17" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" ht="65.25" customHeight="1">
+      <c r="A18" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="13" t="s">
+      <c r="F18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="120">
-      <c r="A8" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="H18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="64.5" customHeight="1">
+      <c r="A19" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="120">
-      <c r="A9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="13" t="s">
+      <c r="H19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="79.5" customHeight="1">
+      <c r="A20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="120">
-      <c r="A10" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="13" t="s">
+      <c r="H20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="78" customHeight="1">
+      <c r="A21" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="90">
-      <c r="A11" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="H21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J21" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="105">
-      <c r="A12" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="105">
-      <c r="A13" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="105">
-      <c r="A14" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="30">
-      <c r="A15" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="30">
-      <c r="A16" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="30">
-      <c r="A17" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="15">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" ht="15">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" ht="15">
-      <c r="A20" s="4"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" ht="15">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="10"/>
+    <row r="22" spans="1:10" ht="15">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="23"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dodanie przypadków dot. edycji adresu do wysyłki
</commit_message>
<xml_diff>
--- a/PrzypadkiUżycia.xlsx
+++ b/PrzypadkiUżycia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="121">
   <si>
     <t>numer ID</t>
   </si>
@@ -422,6 +422,84 @@
 4. W polu "Nowe hasło" wpisz hasło zawierające mniej niż 12 znaków.
 5. Powtórz hasło w polu "Potwierdź nowe hasło".
 6. Kliknij przycisk "Zapisz zmiany".</t>
+  </si>
+  <si>
+    <t>Próba zmiany hasła w przypadku niewypełnienia wymaganych pól.</t>
+  </si>
+  <si>
+    <t>Celem testu jest sprawdzenie zachowania się systemu przy próbie zmiany hasła przy braku wypełnienia wymaganych pól (Imię i Nazwisko).</t>
+  </si>
+  <si>
+    <t>3. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Szczegóły konta".
+3. W polu "Aktualne hasło" wpisz hasło otrzymane na maila wraz z mailem potwierdzającym rejestrację lub swoje zmienione hasło.
+4. W polu "Nowe hasło" wpisz hasło składające się z conajmniej 12 znaków.
+5. Powtórz hasło w polu "Potwierdź nowe hasło".
+6. Pola "Imię" oraz "Nazwisko" pozostaw puste.
+7. Kliknij przycisk "Zapisz zmiany"._x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</t>
+  </si>
+  <si>
+    <t>Komunikat z informacją o konieczności wypełnienia wymaganych pól.</t>
+  </si>
+  <si>
+    <t>Poprawna edycja adresu do wysyłki.</t>
+  </si>
+  <si>
+    <t>Celem testu jest edycja adresu do wysyłki przy zachowaniu poprawnego wypełnienia wymaganych pól.</t>
+  </si>
+  <si>
+    <t>Komunikat o pozytywnej zmianie adresu do wysyłki.</t>
+  </si>
+  <si>
+    <t>Adres do wysyłki został zmieniony.</t>
+  </si>
+  <si>
+    <t>1. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Adresy".
+3. W rubryce "Adres do wysyłki" kliknij "Edytuj".
+4. Wypełnij poprawnie wszystkie wymagane pola formularza.
+5. Kliknij "Zapisz adres".</t>
+  </si>
+  <si>
+    <t>ID 0021</t>
+  </si>
+  <si>
+    <t>ID 0022</t>
+  </si>
+  <si>
+    <t>Próba edycji adresu do wysyłki przy niewypełnieniu wymaganych pól formularza.</t>
+  </si>
+  <si>
+    <t>1. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Adresy".
+3. W rubryce "Adres do wysyłki" kliknij "Edytuj".
+4. Wypełnij pola formularza z losowym pominięciem niektórych z wymaganych pól.
+5. Kliknij "Zapisz adres".</t>
+  </si>
+  <si>
+    <t>Komunikat o wymaganym wypełnieniu danego pola.</t>
+  </si>
+  <si>
+    <t>Adres do wysyłki nie został zmieniony.</t>
+  </si>
+  <si>
+    <t>Próba edycji adresu do wysyłki przy niepoprawnym wypełnieniu pola "Kod pocztowy".</t>
+  </si>
+  <si>
+    <t>Celem testu jest sprawdzenie zachowania się systemu podczas próby edycji adresu do wysyłki przy braku wypełnienia wymaganych pól.</t>
+  </si>
+  <si>
+    <t>Celem testu jest sprawdzenie zachowania się systemu podczas edycji adresu do wysyłki przy błędnym wypełnieniu pola "Kod pocztowy".</t>
+  </si>
+  <si>
+    <t>1. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Adresy".
+3. W rubryce "Adres do wysyłki" kliknij "Edytuj".
+4. Wypełnij pola formularza, w polu "Kod pocztowy" wpisz ciąg znaków składający się z liter.
+5. Kliknij "Zapisz adres".</t>
+  </si>
+  <si>
+    <t>Komunikat o wymaganym poprawnym wypełnieniu pola.</t>
   </si>
 </sst>
 </file>
@@ -1074,11 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13:J13"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1479,69 +1557,133 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30">
+    <row r="13" spans="1:10" ht="135">
       <c r="A13" s="9" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" ht="30">
+      <c r="C13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="75">
       <c r="A14" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" ht="30">
+      <c r="C14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="90">
       <c r="A15" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" ht="30">
+      <c r="C15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="90">
       <c r="A16" s="9" t="s">
         <v>79</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="3"/>
+      <c r="C16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="30">
       <c r="A17" s="9" t="s">
@@ -1559,71 +1701,39 @@
       <c r="I17" s="1"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="65.25" customHeight="1">
+    <row r="18" spans="1:10" ht="30">
       <c r="A18" s="9" t="s">
         <v>84</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="64.5" customHeight="1">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" ht="30">
       <c r="A19" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="79.5" customHeight="1">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" ht="65.25" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>86</v>
       </c>
@@ -1631,10 +1741,10 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>12</v>
@@ -1646,7 +1756,7 @@
         <v>13</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>73</v>
@@ -1655,7 +1765,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="78" customHeight="1">
+    <row r="21" spans="1:10" ht="64.5" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>87</v>
       </c>
@@ -1663,10 +1773,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>12</v>
@@ -1678,7 +1788,7 @@
         <v>13</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>73</v>
@@ -1687,29 +1797,93 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="23"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="8"/>
+    <row r="22" spans="1:10" ht="79.5" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="78" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="23"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dodanie przypadków dot. usuwania produktów z koszyka oraz dodawania produktów do zapakowania
</commit_message>
<xml_diff>
--- a/PrzypadkiUżycia.xlsx
+++ b/PrzypadkiUżycia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="172">
   <si>
     <t>numer ID</t>
   </si>
@@ -357,10 +357,6 @@
     <t>Sprawdzenie poprawności działania systemu dla operacji dodawania produktów do koszyka z poziomu pop-up'u z opisem produktu.</t>
   </si>
   <si>
-    <t>2. Na stronie głównej sklepu wybierz dowolny produkt i kliknij na ikonę lupki. Otworzy się pop-up z opisem produktu.
-2. Kliknij przycisk "Dodaj do koszyka".</t>
-  </si>
-  <si>
     <t>ID 0017</t>
   </si>
   <si>
@@ -500,6 +496,197 @@
   </si>
   <si>
     <t>Komunikat o wymaganym poprawnym wypełnieniu pola.</t>
+  </si>
+  <si>
+    <t>ID 0023</t>
+  </si>
+  <si>
+    <t>ID 0024</t>
+  </si>
+  <si>
+    <t>Poprawna edycja adresu rozliczeniowego.</t>
+  </si>
+  <si>
+    <t>Próba edycji adresu rozliczeniowego przy niewypełnieniu wymaganych pól formularza.</t>
+  </si>
+  <si>
+    <t>Próba edycji adresu rozliczeniowego przy niepoprawnym wypełnieniu pola "Kod pocztowy".</t>
+  </si>
+  <si>
+    <t>Celem testu jest edycja adresu rozliczeniowego przy zachowaniu poprawnego wypełnienia wymaganych pól.</t>
+  </si>
+  <si>
+    <t>Celem testu jest sprawdzenie zachowania się systemu podczas próby edycji adresu rozliczeniowego przy braku wypełnienia wymaganych pól.</t>
+  </si>
+  <si>
+    <t>Celem testu jest sprawdzenie zachowania się systemu podczas edycji adresu rozliczeniowego przy błędnym wypełnieniu pola "Kod pocztowy".</t>
+  </si>
+  <si>
+    <t>1. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Adresy".
+3. W rubryce "Adres rozliczeniowy" kliknij "Edytuj".
+4. Wypełnij pola formularza z losowym pominięciem niektórych z wymaganych pól.
+5. Kliknij "Zapisz adres".</t>
+  </si>
+  <si>
+    <t>1. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Adresy".
+3. W rubryce "Adres rozliczeniowy" kliknij "Edytuj".
+4. Wypełnij poprawnie wszystkie wymagane pola formularza.
+5. Kliknij "Zapisz adres".</t>
+  </si>
+  <si>
+    <t>Komunikat o pozytywnej zmianie adresu rozliczeniowego.</t>
+  </si>
+  <si>
+    <t>Adres rozliczeniowy został zmieniony.</t>
+  </si>
+  <si>
+    <t>Adres rozliczeniowy nie został zmieniony.</t>
+  </si>
+  <si>
+    <t>1. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Adresy".
+3. W rubryce "Adres rozliczeniowy" kliknij "Edytuj".
+4. Wypełnij pola formularza, w polu "Kod pocztowy" wpisz ciąg znaków składający się z liter.
+5. Kliknij "Zapisz adres".</t>
+  </si>
+  <si>
+    <t>2. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Adresy".
+3. W rubryce "Adres rozliczeniowy" kliknij "Edytuj".
+4. Wypełnij pola formularza, w polu "Telefon" wpisz ciąg znaków składający się z mniej niż 9 cyfr lub więcej niż 9 cyfr.
+5. Kliknij "Zapisz adres"._x0000__x0000__x0000__x0000__x0000_</t>
+  </si>
+  <si>
+    <t>Celem testu jest sprawdzenie zachowania się systemu podczas edycji adresu rozliczeniowego przy wypełnieniu pola "Telefon" nieprawidłową liczbą cyfr.</t>
+  </si>
+  <si>
+    <t>Próba edycji adresu rozliczeniowego przy wypełnieniu pola "Telefon" niewłaściwą liczbą cyfr.</t>
+  </si>
+  <si>
+    <t>Próba edycji adresu rozliczeniowego przy wypełnieniu pola "Telefon" niewłaściwym ciągiem znaków.</t>
+  </si>
+  <si>
+    <t>Celem testu jest sprawdzenie zachowania się systemu podczas edycji adresu rozliczeniowego przy wypełnieniu pola "Telefon" niewłaściwym ciągiem znaków składającym się z liter i znaków specjalnych.</t>
+  </si>
+  <si>
+    <t>3. Kliknij ikonę rozwijanego menu, wybierz zakładkę "Moje konto".
+2. Wybierz zakładkę "Adresy".
+3. W rubryce "Adres rozliczeniowy" kliknij "Edytuj".
+4. Wypełnij pola formularza, w polu "Telefon" wpisz ciąg znakównp. 123qaz$%^.
+5. Kliknij "Zapisz zmiany".</t>
+  </si>
+  <si>
+    <t>Komunikat o niepoprawnym wypełnieniu pola.</t>
+  </si>
+  <si>
+    <t>Komunikat o niepoprawnym wypełnieniu pola..</t>
+  </si>
+  <si>
+    <t>Komunikat o konieczności wypełnienia danego pola.</t>
+  </si>
+  <si>
+    <t>ID 0025</t>
+  </si>
+  <si>
+    <t>ID 0026</t>
+  </si>
+  <si>
+    <t>ID 0027</t>
+  </si>
+  <si>
+    <t>ID 0028</t>
+  </si>
+  <si>
+    <t>ID 0029</t>
+  </si>
+  <si>
+    <t>Dodawanie produktu do zapakowania na prezent - przycisk.</t>
+  </si>
+  <si>
+    <t>Sprawdzenie poprawności działania systemu dla operacji dodawania produktów do zapakowania na prezent przy użyciu przycisku.</t>
+  </si>
+  <si>
+    <t>1. Na stronie głównej sklepu wybierz dowolny produkt i kliknij na ikonę lupki. Otworzy się pop-up z opisem produktu.
+2. Kliknij przycisk "Dodaj do koszyka".</t>
+  </si>
+  <si>
+    <t>Dodawanie produktu do zapakowania na prezent z podstrony produktu.</t>
+  </si>
+  <si>
+    <t>Sprawdzenie poprawności działania systemu dla operacji dodawania produktów do zapakowania z podstrony z opisem produktu .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Na stronie głównej sklepu wybierz dowolny produkt i dodaj go do zapakowania używając przycisku "Zapakuj" pod miniaturą produktu.
+2. Wybierz wzór opakowania produktu. Kliknij przycisk "Dalej".
+3. Opcjonalnie wypełnij pola "Dedykacja" oraz "Nadawca".
+4. Zamknij okno klikając krzyżyk.
+</t>
+  </si>
+  <si>
+    <t>Po zamknięciu okna ponownie wyświetlona zostaje strona produktu.</t>
+  </si>
+  <si>
+    <t>Produkt dodany do zapakowania na prezent.</t>
+  </si>
+  <si>
+    <t>Dodawanie produktu do zapakowania na prezent z poziomu pop-up'u produktu.</t>
+  </si>
+  <si>
+    <t>Sprawdzenie poprawności działania systemu dla operacji dodawania produktów do zapakowania z poziomu pop-up'u z opisem produktu.</t>
+  </si>
+  <si>
+    <t>1. Na stronie głównej sklepu wybierz dowolny produkt i kliknij w jego miniaturę.
+2. Dodaj go do zapakowania używając przycisku "Zapakuj".
+3. Wybierz wzór opakowania produktu. Kliknij przycisk "Dalej".
+4. Opcjonalnie wypełnij pola "Dedykacja" oraz "Nadawca".
+5. Zamknij okno klikając symbol krzyżyka._x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</t>
+  </si>
+  <si>
+    <t>1. Na stronie głównej sklepu wybierz dowolny produkt i kliknij na ikonę lupki. Otworzy się pop-up z opisem produktu.
+2. Dodaj go do zapakowania używając przycisku "Zapakuj".
+3. Wybierz wzór opakowania produktu. Kliknij przycisk "Dalej".
+4. Opcjonalnie wypełnij pola "Dedykacja" oraz "Nadawca. 
+5. Zamknij okno klikając symbol krzyżyka._x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000__x0000_</t>
+  </si>
+  <si>
+    <t>ID 0030</t>
+  </si>
+  <si>
+    <t>ID 0031</t>
+  </si>
+  <si>
+    <t>ID 0032</t>
+  </si>
+  <si>
+    <t>ID 0033</t>
+  </si>
+  <si>
+    <t>Usuwanie produktu z koszyka standardowego.</t>
+  </si>
+  <si>
+    <t>1. Na stronie głównej sklepu kliknij ikonę koszyka sklepowego (w górnej części strony, po prawej stronie).
+2. Usuń produkt z koszyka klikając przycisk z symbolem krzyżyka po prawej stronie.</t>
+  </si>
+  <si>
+    <t>Komunikat o usunięciu produktu z koszyka.</t>
+  </si>
+  <si>
+    <t>Produkt został usunięty z koszyka.</t>
+  </si>
+  <si>
+    <t>Usuwanie produktu z koszyka produktów do zapakowania na prezent.</t>
+  </si>
+  <si>
+    <t>Sprawdzenie poprawności działania systemu dla operacji usuwania produktów z koszyka produktów do zapakowania na prezent.</t>
+  </si>
+  <si>
+    <t>Sprawdzenie poprawności działania systemu dla operacji usuwania produktów z koszyka standardowego.</t>
+  </si>
+  <si>
+    <t>1. Na stronie głównej sklepu kliknij ikonę prezentu (w prawym górnym rogu strony).
+2. Usuń produkt z koszyka klikając przycisk z symbolem krzyżyka po prawej stronie.</t>
   </si>
 </sst>
 </file>
@@ -552,7 +739,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -562,6 +749,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,7 +927,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -750,7 +943,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -760,23 +953,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -787,14 +982,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -807,9 +999,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -821,9 +1010,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -840,22 +1026,88 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1152,256 +1404,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.25" customWidth="1"/>
-    <col min="2" max="2" width="10.875" customWidth="1"/>
-    <col min="3" max="3" width="21.375" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="26.75" customWidth="1"/>
-    <col min="7" max="7" width="27.625" customWidth="1"/>
-    <col min="8" max="8" width="58.125" customWidth="1"/>
-    <col min="9" max="9" width="23.625" customWidth="1"/>
-    <col min="10" max="10" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="7.25" style="20" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="21.375" style="20" customWidth="1"/>
+    <col min="4" max="4" width="27" style="20" customWidth="1"/>
+    <col min="5" max="5" width="10" style="20" customWidth="1"/>
+    <col min="6" max="6" width="26.75" style="20" customWidth="1"/>
+    <col min="7" max="7" width="27.625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="58.125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="23.625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="63" customHeight="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:10" ht="60">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="13" t="s">
+      <c r="I2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="77.25" customHeight="1">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:10" ht="75">
+      <c r="A3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="G3" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="78.75" customHeight="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:10" ht="75">
+      <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="G4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="21" t="s">
         <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="81.75" customHeight="1">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:10" ht="75">
+      <c r="A5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="79.5" customHeight="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:10" ht="75">
+      <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="G6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="22" t="s">
         <v>62</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="96" customHeight="1">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:10" ht="90">
+      <c r="A7" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="G7" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="30" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="95.25" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:10" ht="90">
+      <c r="A8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1413,59 +1666,59 @@
       <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="22" t="s">
         <v>48</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="95.25" customHeight="1">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:10" ht="90">
+      <c r="A9" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="G9" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="95.25" customHeight="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:10" ht="90">
+      <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1477,413 +1730,749 @@
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="G10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="22" t="s">
         <v>57</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="155.25" customHeight="1">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:10" ht="150">
+      <c r="A11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="105">
+      <c r="A12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="108.75" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="F12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="123" customHeight="1">
+      <c r="A13" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="135">
-      <c r="A13" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="75">
+      <c r="A14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="75">
-      <c r="A14" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>109</v>
+      <c r="F14" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="22" t="s">
+        <v>108</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="15" spans="1:10" ht="90">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="I15" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="J15" s="30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="90">
+      <c r="A16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="90">
-      <c r="A16" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="F16" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30">
-      <c r="A17" s="9" t="s">
+      <c r="J16" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="75">
+      <c r="A17" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" ht="30">
-      <c r="A18" s="9" t="s">
+      <c r="B17" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="90">
+      <c r="A18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="90">
+      <c r="A19" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" ht="30">
-      <c r="A19" s="9" t="s">
+      <c r="B19" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="90">
+      <c r="A20" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" ht="65.25" customHeight="1">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="105">
+      <c r="A21" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B21" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="J21" s="30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="60">
+      <c r="A22" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="64.5" customHeight="1">
-      <c r="A21" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="79.5" customHeight="1">
-      <c r="A22" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>70</v>
+      <c r="G22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="78" customHeight="1">
-      <c r="A23" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="1" t="s">
+    <row r="23" spans="1:10" ht="60">
+      <c r="A23" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="75">
+      <c r="A24" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="75">
+      <c r="A25" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D25" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E25" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F25" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I23" s="1" t="s">
+      <c r="G25" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="I25" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J25" s="30" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="23"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="8"/>
+    <row r="26" spans="1:10" ht="79.5" customHeight="1">
+      <c r="A26" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="90">
+      <c r="A27" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="J27" s="30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="90">
+      <c r="A28" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="72" customHeight="1">
+      <c r="A29" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="J29" s="35" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="75">
+      <c r="A30" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="I30" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="J30" s="42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="30">
+      <c r="A31" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="35"/>
+    </row>
+    <row r="32" spans="1:10" ht="30">
+      <c r="A32" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="16"/>
+    </row>
+    <row r="33" spans="1:10" ht="30">
+      <c r="A33" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="35"/>
+    </row>
+    <row r="34" spans="1:10" ht="30">
+      <c r="A34" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="1:10" ht="15">
+      <c r="A35" s="19"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="16"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>